<commit_message>
Update data import library
</commit_message>
<xml_diff>
--- a/curation/templates/TemplateColumns2Models.xlsx
+++ b/curation/templates/TemplateColumns2Models.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lg10/Workspace/git/fork/PGS_import/curation/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lg10/Workspace/git/fork/PGS_curation/curation/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FAD6132-0533-4B40-9E90-DB6688F49393}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A01F8844-61CF-0F45-963C-CA3656C02FDF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="1520" windowWidth="28800" windowHeight="16260" activeTab="1" xr2:uid="{B0CC4535-7E6E-584E-9FDE-AD77876CF244}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16260" xr2:uid="{B0CC4535-7E6E-584E-9FDE-AD77876CF244}"/>
   </bookViews>
   <sheets>
     <sheet name="Version" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="155">
   <si>
     <t>Sheet</t>
   </si>
@@ -1184,6 +1184,15 @@
   </si>
   <si>
     <t>Cohort Name</t>
+  </si>
+  <si>
+    <t>Replaced by "source_DOI" when the value is not a PubMed ID</t>
+  </si>
+  <si>
+    <t>Other/previous Names</t>
+  </si>
+  <si>
+    <t>name_others</t>
   </si>
 </sst>
 </file>
@@ -1310,7 +1319,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -1656,11 +1665,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1787,6 +1818,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2103,8 +2136,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ADA4E12-E6DC-DD44-8C1B-013CCB4D7782}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2114,7 +2147,7 @@
         <v>149</v>
       </c>
       <c r="B1">
-        <v>7</v>
+        <v>7.1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -2122,7 +2155,7 @@
         <v>150</v>
       </c>
       <c r="B2" s="61">
-        <v>44337</v>
+        <v>44662</v>
       </c>
     </row>
   </sheetData>
@@ -2134,8 +2167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41FDEE91-4AEE-FD49-8B2B-E0D2B4B6944F}">
   <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2586,6 +2619,9 @@
         <v>136</v>
       </c>
       <c r="F23" s="30"/>
+      <c r="G23" s="38" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="24" spans="1:7" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
@@ -2603,9 +2639,7 @@
       <c r="E24" s="25" t="s">
         <v>135</v>
       </c>
-      <c r="F24" s="30" t="s">
-        <v>139</v>
-      </c>
+      <c r="F24" s="30"/>
     </row>
     <row r="25" spans="1:7" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
@@ -3069,26 +3103,42 @@
       </c>
     </row>
     <row r="50" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="47" t="s">
+      <c r="A50" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B50" s="58" t="s">
+      <c r="B50" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="C50" s="47" t="s">
+      <c r="C50" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D50" s="47" t="s">
+      <c r="D50" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E50" s="26" t="s">
-        <v>136</v>
-      </c>
-      <c r="F50" s="26"/>
-      <c r="G50" s="59"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B51" s="38"/>
+      <c r="E50" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="F50" s="25"/>
+      <c r="G50" s="62"/>
+    </row>
+    <row r="51" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A51" s="47" t="s">
+        <v>36</v>
+      </c>
+      <c r="B51" s="58" t="s">
+        <v>153</v>
+      </c>
+      <c r="C51" s="47" t="s">
+        <v>72</v>
+      </c>
+      <c r="D51" s="47" t="s">
+        <v>154</v>
+      </c>
+      <c r="E51" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="F51" s="63"/>
+      <c r="G51" s="56"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B52" s="38"/>

</xml_diff>

<commit_message>
Fetch the EFO names, to check that they match the given EFO IDs and improve the error reports
</commit_message>
<xml_diff>
--- a/curation/templates/TemplateColumns2Models.xlsx
+++ b/curation/templates/TemplateColumns2Models.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lg10/Workspace/git/fork/PGS_curation/curation/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A01F8844-61CF-0F45-963C-CA3656C02FDF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AFE0CC8-B159-BF44-8420-ABEC4F8CD4D9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16260" xr2:uid="{B0CC4535-7E6E-584E-9FDE-AD77876CF244}"/>
+    <workbookView xWindow="32820" yWindow="2860" windowWidth="28800" windowHeight="16120" activeTab="1" xr2:uid="{B0CC4535-7E6E-584E-9FDE-AD77876CF244}"/>
   </bookViews>
   <sheets>
     <sheet name="Version" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="157">
   <si>
     <t>Sheet</t>
   </si>
@@ -1193,6 +1193,51 @@
   </si>
   <si>
     <t>name_others</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">EFO Names
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(Names of suggested ontology terms -</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>can ignore: it will be extracted by curators</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>trait_efo_name</t>
   </si>
 </sst>
 </file>
@@ -1319,7 +1364,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -1687,11 +1732,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1820,6 +1880,9 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2136,7 +2199,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ADA4E12-E6DC-DD44-8C1B-013CCB4D7782}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -2165,10 +2228,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41FDEE91-4AEE-FD49-8B2B-E0D2B4B6944F}">
-  <dimension ref="A1:G60"/>
+  <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="E57" sqref="E57"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2415,14 +2478,14 @@
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="7" t="s">
-        <v>12</v>
+      <c r="B13" s="64" t="s">
+        <v>155</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>44</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>49</v>
+        <v>156</v>
       </c>
       <c r="E13" s="25" t="s">
         <v>136</v>
@@ -2435,32 +2498,34 @@
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="8" t="s">
-        <v>13</v>
+      <c r="B14" s="7" t="s">
+        <v>12</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>44</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E14" s="25" t="s">
         <v>136</v>
       </c>
-      <c r="F14" s="30"/>
+      <c r="F14" s="30" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="15" spans="1:7" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>86</v>
+        <v>13</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>44</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>87</v>
+        <v>50</v>
       </c>
       <c r="E15" s="25" t="s">
         <v>136</v>
@@ -2472,84 +2537,83 @@
         <v>16</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>14</v>
+        <v>86</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>44</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>51</v>
+        <v>87</v>
       </c>
       <c r="E16" s="25" t="s">
-        <v>135</v>
-      </c>
-      <c r="F16" s="30" t="s">
-        <v>139</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="F16" s="30"/>
     </row>
     <row r="17" spans="1:7" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="16" t="s">
-        <v>15</v>
+      <c r="B17" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>44</v>
       </c>
       <c r="D17" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="F17" s="30" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E17" s="37" t="s">
-        <v>136</v>
-      </c>
-      <c r="F17" s="37"/>
-      <c r="G17" s="39"/>
-    </row>
-    <row r="18" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="52" t="s">
+      <c r="E18" s="37" t="s">
+        <v>136</v>
+      </c>
+      <c r="F18" s="37"/>
+      <c r="G18" s="39"/>
+    </row>
+    <row r="19" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="53" t="s">
+      <c r="B19" s="53" t="s">
         <v>133</v>
       </c>
-      <c r="C18" s="47" t="s">
+      <c r="C19" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="47" t="s">
+      <c r="D19" s="47" t="s">
         <v>132</v>
       </c>
-      <c r="E18" s="52" t="s">
-        <v>136</v>
-      </c>
-      <c r="F18" s="49"/>
-      <c r="G18" s="49"/>
-    </row>
-    <row r="19" spans="1:7" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="51" t="s">
-        <v>88</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D19" s="1"/>
-      <c r="E19" s="25" t="s">
-        <v>136</v>
-      </c>
-      <c r="F19" s="30"/>
-      <c r="G19" s="38" t="s">
-        <v>55</v>
-      </c>
+      <c r="E19" s="52" t="s">
+        <v>136</v>
+      </c>
+      <c r="F19" s="49"/>
+      <c r="G19" s="49"/>
     </row>
     <row r="20" spans="1:7" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="17" t="s">
-        <v>18</v>
+      <c r="B20" s="51" t="s">
+        <v>88</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>53</v>
@@ -2558,11 +2622,9 @@
       <c r="E20" s="25" t="s">
         <v>136</v>
       </c>
-      <c r="F20" s="30" t="s">
-        <v>139</v>
-      </c>
+      <c r="F20" s="30"/>
       <c r="G20" s="38" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2570,7 +2632,7 @@
         <v>17</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>53</v>
@@ -2579,9 +2641,11 @@
       <c r="E21" s="25" t="s">
         <v>136</v>
       </c>
-      <c r="F21" s="30"/>
+      <c r="F21" s="30" t="s">
+        <v>139</v>
+      </c>
       <c r="G21" s="38" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2589,70 +2653,71 @@
         <v>17</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>58</v>
-      </c>
+      <c r="D22" s="1"/>
       <c r="E22" s="25" t="s">
         <v>136</v>
       </c>
       <c r="F22" s="30"/>
+      <c r="G22" s="38" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="23" spans="1:7" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>53</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E23" s="25" t="s">
         <v>136</v>
       </c>
       <c r="F23" s="30"/>
-      <c r="G23" s="38" t="s">
-        <v>152</v>
-      </c>
     </row>
     <row r="24" spans="1:7" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B24" s="18" t="s">
-        <v>22</v>
+      <c r="B24" s="17" t="s">
+        <v>21</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>53</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E24" s="25" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F24" s="30"/>
+      <c r="G24" s="38" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="25" spans="1:7" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>53</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E25" s="25" t="s">
         <v>135</v>
@@ -2664,13 +2729,13 @@
         <v>17</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>53</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E26" s="25" t="s">
         <v>135</v>
@@ -2681,17 +2746,17 @@
       <c r="A27" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B27" s="19" t="s">
-        <v>25</v>
+      <c r="B27" s="18" t="s">
+        <v>24</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>53</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E27" s="25" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F27" s="30"/>
     </row>
@@ -2699,41 +2764,39 @@
       <c r="A28" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="22" t="s">
-        <v>124</v>
+      <c r="B28" s="19" t="s">
+        <v>25</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>53</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>126</v>
+        <v>63</v>
       </c>
       <c r="E28" s="25" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F28" s="30"/>
-      <c r="G28" s="3" t="s">
-        <v>127</v>
-      </c>
     </row>
     <row r="29" spans="1:7" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B29" s="20" t="s">
-        <v>26</v>
+      <c r="B29" s="22" t="s">
+        <v>124</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>53</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>64</v>
+        <v>126</v>
       </c>
       <c r="E29" s="25" t="s">
         <v>136</v>
       </c>
-      <c r="F29" s="30" t="s">
-        <v>139</v>
+      <c r="F29" s="30"/>
+      <c r="G29" s="3" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2741,31 +2804,33 @@
         <v>17</v>
       </c>
       <c r="B30" s="20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>53</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E30" s="25" t="s">
         <v>136</v>
       </c>
-      <c r="F30" s="30"/>
+      <c r="F30" s="30" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="31" spans="1:7" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B31" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>53</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E31" s="25" t="s">
         <v>136</v>
@@ -2777,13 +2842,13 @@
         <v>17</v>
       </c>
       <c r="B32" s="20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>53</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E32" s="25" t="s">
         <v>136</v>
@@ -2794,14 +2859,14 @@
       <c r="A33" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B33" s="21" t="s">
-        <v>30</v>
+      <c r="B33" s="20" t="s">
+        <v>29</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>53</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="E33" s="25" t="s">
         <v>136</v>
@@ -2812,90 +2877,87 @@
       <c r="A34" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B34" s="23" t="s">
-        <v>141</v>
+      <c r="B34" s="21" t="s">
+        <v>30</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>53</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>125</v>
+        <v>84</v>
       </c>
       <c r="E34" s="25" t="s">
         <v>136</v>
       </c>
       <c r="F34" s="30"/>
-      <c r="G34" s="3" t="s">
-        <v>127</v>
-      </c>
     </row>
     <row r="35" spans="1:7" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B35" s="17" t="s">
-        <v>31</v>
+      <c r="B35" s="23" t="s">
+        <v>141</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>53</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>69</v>
+        <v>125</v>
       </c>
       <c r="E35" s="25" t="s">
         <v>136</v>
       </c>
       <c r="F35" s="30"/>
       <c r="G35" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B36" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E36" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="F36" s="30"/>
+      <c r="G36" s="3" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="47" t="s">
+    <row r="37" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="B36" s="55" t="s">
+      <c r="B37" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="C36" s="47" t="s">
+      <c r="C37" s="47" t="s">
         <v>53</v>
       </c>
-      <c r="D36" s="47" t="s">
+      <c r="D37" s="47" t="s">
         <v>68</v>
       </c>
-      <c r="E36" s="26" t="s">
-        <v>136</v>
-      </c>
-      <c r="F36" s="26"/>
-      <c r="G36" s="56"/>
-    </row>
-    <row r="37" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B37" s="54" t="s">
-        <v>81</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D37" s="1"/>
-      <c r="E37" s="25" t="s">
-        <v>136</v>
-      </c>
-      <c r="F37" s="30" t="s">
-        <v>139</v>
-      </c>
-      <c r="G37" s="3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E37" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="F37" s="26"/>
+      <c r="G37" s="56"/>
+    </row>
+    <row r="38" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B38" s="5" t="s">
-        <v>38</v>
+      <c r="B38" s="54" t="s">
+        <v>81</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>70</v>
@@ -2908,73 +2970,78 @@
         <v>139</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B39" s="11" t="s">
-        <v>121</v>
+      <c r="B39" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D39" s="1" t="s">
-        <v>123</v>
-      </c>
+      <c r="D39" s="1"/>
       <c r="E39" s="25" t="s">
         <v>136</v>
       </c>
       <c r="F39" s="30" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G39" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B40" s="41" t="s">
-        <v>34</v>
+      <c r="B40" s="11" t="s">
+        <v>121</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>70</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E40" s="28"/>
-      <c r="F40" s="32"/>
+        <v>123</v>
+      </c>
+      <c r="E40" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="F40" s="30" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="41" spans="1:7" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B41" s="42" t="s">
-        <v>35</v>
+      <c r="B41" s="41" t="s">
+        <v>34</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D41" s="38" t="s">
-        <v>76</v>
-      </c>
-      <c r="E41" s="27"/>
-      <c r="F41" s="31"/>
+      <c r="D41" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E41" s="28"/>
+      <c r="F41" s="32"/>
     </row>
     <row r="42" spans="1:7" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B42" s="43" t="s">
-        <v>142</v>
+      <c r="B42" s="42" t="s">
+        <v>35</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D42" s="2" t="s">
-        <v>78</v>
+      <c r="D42" s="38" t="s">
+        <v>76</v>
       </c>
       <c r="E42" s="27"/>
       <c r="F42" s="31"/>
@@ -2983,30 +3050,30 @@
       <c r="A43" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B43" s="41" t="s">
-        <v>143</v>
+      <c r="B43" s="43" t="s">
+        <v>142</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D43" s="38" t="s">
-        <v>74</v>
-      </c>
-      <c r="E43" s="25"/>
-      <c r="F43" s="30"/>
+      <c r="D43" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E43" s="27"/>
+      <c r="F43" s="31"/>
     </row>
     <row r="44" spans="1:7" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B44" s="43" t="s">
-        <v>144</v>
+      <c r="B44" s="41" t="s">
+        <v>143</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>70</v>
       </c>
       <c r="D44" s="38" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E44" s="25"/>
       <c r="F44" s="30"/>
@@ -3015,133 +3082,146 @@
       <c r="A45" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B45" s="41" t="s">
-        <v>145</v>
+      <c r="B45" s="43" t="s">
+        <v>144</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D45" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E45" s="39"/>
-      <c r="F45" s="39"/>
-      <c r="G45" s="39"/>
+      <c r="D45" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="E45" s="25"/>
+      <c r="F45" s="30"/>
     </row>
     <row r="46" spans="1:7" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B46" s="43" t="s">
-        <v>146</v>
+      <c r="B46" s="41" t="s">
+        <v>145</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>70</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E46" s="39"/>
       <c r="F46" s="39"/>
       <c r="G46" s="39"/>
     </row>
-    <row r="47" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B47" s="6" t="s">
-        <v>39</v>
+      <c r="B47" s="43" t="s">
+        <v>146</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>70</v>
       </c>
       <c r="D47" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E47" s="39"/>
+      <c r="F47" s="39"/>
+      <c r="G47" s="39"/>
+    </row>
+    <row r="48" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D48" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E47" s="25" t="s">
-        <v>136</v>
-      </c>
-      <c r="F47" s="30"/>
-    </row>
-    <row r="48" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="47" t="s">
+      <c r="E48" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="F48" s="30"/>
+    </row>
+    <row r="49" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="B48" s="57" t="s">
+      <c r="B49" s="57" t="s">
         <v>40</v>
       </c>
-      <c r="C48" s="47" t="s">
+      <c r="C49" s="47" t="s">
         <v>70</v>
       </c>
-      <c r="D48" s="47" t="s">
+      <c r="D49" s="47" t="s">
         <v>80</v>
       </c>
-      <c r="E48" s="26" t="s">
-        <v>136</v>
-      </c>
-      <c r="F48" s="26"/>
-      <c r="G48" s="59"/>
-    </row>
-    <row r="49" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E49" s="25" t="s">
-        <v>136</v>
-      </c>
-      <c r="F49" s="30" t="s">
-        <v>139</v>
-      </c>
+      <c r="E49" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="F49" s="26"/>
+      <c r="G49" s="59"/>
     </row>
     <row r="50" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>151</v>
+        <v>37</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>72</v>
       </c>
       <c r="D50" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E50" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="F50" s="30" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D51" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E50" s="25" t="s">
-        <v>136</v>
-      </c>
-      <c r="F50" s="25"/>
-      <c r="G50" s="62"/>
-    </row>
-    <row r="51" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A51" s="47" t="s">
+      <c r="E51" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="F51" s="25"/>
+      <c r="G51" s="62"/>
+    </row>
+    <row r="52" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A52" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="B51" s="58" t="s">
+      <c r="B52" s="58" t="s">
         <v>153</v>
       </c>
-      <c r="C51" s="47" t="s">
+      <c r="C52" s="47" t="s">
         <v>72</v>
       </c>
-      <c r="D51" s="47" t="s">
+      <c r="D52" s="47" t="s">
         <v>154</v>
       </c>
-      <c r="E51" s="26" t="s">
-        <v>136</v>
-      </c>
-      <c r="F51" s="63"/>
-      <c r="G51" s="56"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B52" s="38"/>
+      <c r="E52" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="F52" s="63"/>
+      <c r="G52" s="56"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B53" s="38"/>
@@ -3149,10 +3229,10 @@
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B54" s="38"/>
     </row>
-    <row r="55" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B55" s="38"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B56" s="38"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
@@ -3166,6 +3246,9 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B60" s="38"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B61" s="38"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>